<commit_message>
Add results on mito proteome constraint
</commit_message>
<xml_diff>
--- a/application/input/pathways.xlsx
+++ b/application/input/pathways.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="219">
   <si>
     <t xml:space="preserve">product</t>
   </si>
@@ -671,6 +671,15 @@
   </si>
   <si>
     <t xml:space="preserve">MET-skm_e --&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibutoh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RXNADD-IBUTOH1_FWD-SPONT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MET-3mob_m --&gt; MET-3mob_c</t>
   </si>
 </sst>
 </file>
@@ -794,12 +803,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F97"/>
+  <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A56" activeCellId="0" sqref="A56"/>
+      <selection pane="bottomLeft" activeCell="B99" activeCellId="0" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2176,6 +2185,20 @@
         <v>215</v>
       </c>
     </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C98" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F98" s="0" t="s">
+        <v>218</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="B1:F1"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>